<commit_message>
Book Package: total Price Function
</commit_message>
<xml_diff>
--- a/Tourism/DB.xlsx
+++ b/Tourism/DB.xlsx
@@ -12,12 +12,14 @@
     <sheet r:id="rId5" sheetId="3" name="category_management_tbl"/>
     <sheet r:id="rId6" sheetId="4" name="member_signup_tbl"/>
     <sheet r:id="rId7" sheetId="5" name="package_management_tbl"/>
+    <sheet r:id="rId8" sheetId="6" name="booking_contact_details_tbl"/>
   </sheets>
   <definedNames>
-    <definedName name="admin_login_tbl">admin_login_tbl!$A$1:$C$2</definedName>
-    <definedName name="category_management_tbl">category_management_tbl!$A$1:$B$3</definedName>
-    <definedName name="member_signup_tbl">member_signup_tbl!$A$1:$K$2</definedName>
+    <definedName name="admin_login_tbl">admin_login_tbl!$A$1:$C$5</definedName>
+    <definedName name="category_management_tbl">category_management_tbl!$A$1:$B$12</definedName>
+    <definedName name="member_signup_tbl">member_signup_tbl!$A$1:$K$8</definedName>
     <definedName name="package_management_tbl">package_management_tbl!$A$1:$F$1</definedName>
+    <definedName name="booking_contact_details_tbl">booking_contact_details_tbl!$A$1:$F$2</definedName>
   </definedNames>
   <calcPr calcId="162913" fullCalcOnLoad="true"/>
   <extLst>
@@ -351,7 +353,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -386,6 +388,23 @@
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
+        <is>
+          <t>Hetvee Sakaria</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>hetvee_sakaria</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>Hetu@2001</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
         <is>
           <t>Hetvee Sakaria</t>
         </is>
@@ -400,7 +419,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -427,6 +446,120 @@
     </row>
     <row outlineLevel="0" r="3">
       <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Domestic Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>Ritu Agarwal</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>2008-06-10</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>54879672315</t>
+        </is>
+      </c>
+      <c r="D4" s="0" t="inlineStr">
+        <is>
+          <t>rituagarwal@gmail.com</t>
+        </is>
+      </c>
+      <c r="E4" s="0" t="inlineStr">
+        <is>
+          <t>Gujarat</t>
+        </is>
+      </c>
+      <c r="F4" s="0" t="inlineStr">
+        <is>
+          <t>Gandhinagar</t>
+        </is>
+      </c>
+      <c r="G4" s="0" t="inlineStr">
+        <is>
+          <t>345003</t>
+        </is>
+      </c>
+      <c r="H4" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K4" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>National Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>Domestic Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>International Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>National Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="9">
+      <c r="B9" s="0" t="inlineStr">
+        <is>
+          <t>Domestic Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="10">
+      <c r="B10" s="0" t="inlineStr">
+        <is>
+          <t>International Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="11">
+      <c r="B11" s="0" t="inlineStr">
+        <is>
+          <t>National Packages</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="12">
+      <c r="B12" s="0" t="inlineStr">
         <is>
           <t>Domestic Packages</t>
         </is>
@@ -441,7 +574,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="false"/>
   </sheetViews>
@@ -512,27 +645,27 @@
       </c>
       <c r="B2" s="0" t="inlineStr">
         <is>
-          <t>1996-02-13</t>
+          <t>joepatrik@gmail.com</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>6935478966</t>
+          <t>35000</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>joepatrik@gmail.com</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>4</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>Jaipur</t>
+          <t>No thank u</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
@@ -559,6 +692,296 @@
       <c r="K2" s="0" t="inlineStr">
         <is>
           <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>Joe Patrik</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>1996-02-13</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>6935478966</t>
+        </is>
+      </c>
+      <c r="D3" s="0" t="inlineStr">
+        <is>
+          <t>joepatrik@gmail.com</t>
+        </is>
+      </c>
+      <c r="E3" s="0" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="F3" s="0" t="inlineStr">
+        <is>
+          <t>Jaipur</t>
+        </is>
+      </c>
+      <c r="G3" s="0" t="inlineStr">
+        <is>
+          <t>370081</t>
+        </is>
+      </c>
+      <c r="H3" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K3" s="0" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="5">
+      <c r="A5" s="0" t="inlineStr">
+        <is>
+          <t>Joe Patrik</t>
+        </is>
+      </c>
+      <c r="B5" s="0" t="inlineStr">
+        <is>
+          <t>1996-02-13</t>
+        </is>
+      </c>
+      <c r="C5" s="0" t="inlineStr">
+        <is>
+          <t>6935478966</t>
+        </is>
+      </c>
+      <c r="D5" s="0" t="inlineStr">
+        <is>
+          <t>joepatrik@gmail.com</t>
+        </is>
+      </c>
+      <c r="E5" s="0" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="F5" s="0" t="inlineStr">
+        <is>
+          <t>Jaipur</t>
+        </is>
+      </c>
+      <c r="G5" s="0" t="inlineStr">
+        <is>
+          <t>370081</t>
+        </is>
+      </c>
+      <c r="H5" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K5" s="0" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="6">
+      <c r="A6" s="0" t="inlineStr">
+        <is>
+          <t>Ritu Agarwal</t>
+        </is>
+      </c>
+      <c r="B6" s="0" t="inlineStr">
+        <is>
+          <t>2008-06-10</t>
+        </is>
+      </c>
+      <c r="C6" s="0" t="inlineStr">
+        <is>
+          <t>54879672315</t>
+        </is>
+      </c>
+      <c r="D6" s="0" t="inlineStr">
+        <is>
+          <t>rituagarwal@gmail.com</t>
+        </is>
+      </c>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t>Gujarat</t>
+        </is>
+      </c>
+      <c r="F6" s="0" t="inlineStr">
+        <is>
+          <t>Gandhinagar</t>
+        </is>
+      </c>
+      <c r="G6" s="0" t="inlineStr">
+        <is>
+          <t>345003</t>
+        </is>
+      </c>
+      <c r="H6" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K6" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="7">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Joe Patrik</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="inlineStr">
+        <is>
+          <t>1996-02-13</t>
+        </is>
+      </c>
+      <c r="C7" s="0" t="inlineStr">
+        <is>
+          <t>6935478966</t>
+        </is>
+      </c>
+      <c r="D7" s="0" t="inlineStr">
+        <is>
+          <t>joepatrik@gmail.com</t>
+        </is>
+      </c>
+      <c r="E7" s="0" t="inlineStr">
+        <is>
+          <t>Rajasthan</t>
+        </is>
+      </c>
+      <c r="F7" s="0" t="inlineStr">
+        <is>
+          <t>Jaipur</t>
+        </is>
+      </c>
+      <c r="G7" s="0" t="inlineStr">
+        <is>
+          <t>370081</t>
+        </is>
+      </c>
+      <c r="H7" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K7" s="0" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="8">
+      <c r="A8" s="0" t="inlineStr">
+        <is>
+          <t>Ritu Agarwal</t>
+        </is>
+      </c>
+      <c r="B8" s="0" t="inlineStr">
+        <is>
+          <t>2008-06-10</t>
+        </is>
+      </c>
+      <c r="C8" s="0" t="inlineStr">
+        <is>
+          <t>54879672315</t>
+        </is>
+      </c>
+      <c r="D8" s="0" t="inlineStr">
+        <is>
+          <t>rituagarwal@gmail.com</t>
+        </is>
+      </c>
+      <c r="E8" s="0" t="inlineStr">
+        <is>
+          <t>Gujarat</t>
+        </is>
+      </c>
+      <c r="F8" s="0" t="inlineStr">
+        <is>
+          <t>Gandhinagar</t>
+        </is>
+      </c>
+      <c r="G8" s="0" t="inlineStr">
+        <is>
+          <t>345003</t>
+        </is>
+      </c>
+      <c r="H8" s="0" t="inlineStr">
+        <is>
+          <t>Pratik Colony, Near Yash Complex _x000d_
+SG Highway, Jaipur, Rajasthan</t>
+        </is>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
+        <is>
+          <t>123456</t>
+        </is>
+      </c>
+      <c r="K8" s="0" t="inlineStr">
+        <is>
+          <t>pending</t>
         </is>
       </c>
     </row>
@@ -614,4 +1037,85 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" rightToLeft="false"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetData>
+    <row outlineLevel="0" r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B1" s="0" t="inlineStr">
+        <is>
+          <t>email</t>
+        </is>
+      </c>
+      <c r="C1" s="0" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="D1" s="0" t="inlineStr">
+        <is>
+          <t>total_days</t>
+        </is>
+      </c>
+      <c r="E1" s="0" t="inlineStr">
+        <is>
+          <t>total_member</t>
+        </is>
+      </c>
+      <c r="F1" s="0" t="inlineStr">
+        <is>
+          <t>special_request</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="3">
+      <c r="A3" s="0" t="inlineStr">
+        <is>
+          <t>hetvee_sakaria</t>
+        </is>
+      </c>
+      <c r="B3" s="0" t="inlineStr">
+        <is>
+          <t>Hetu@2001</t>
+        </is>
+      </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t>Hetvee Sakaria</t>
+        </is>
+      </c>
+    </row>
+    <row outlineLevel="0" r="4">
+      <c r="A4" s="0" t="inlineStr">
+        <is>
+          <t>hetvee_sakaria</t>
+        </is>
+      </c>
+      <c r="B4" s="0" t="inlineStr">
+        <is>
+          <t>Hetu@2001</t>
+        </is>
+      </c>
+      <c r="C4" s="0" t="inlineStr">
+        <is>
+          <t>Hetvee Sakaria</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>